<commit_message>
Updates to 2D box model spreadsheet
</commit_message>
<xml_diff>
--- a/Working/HW2/HW_02_visualization_example.xlsx
+++ b/Working/HW2/HW_02_visualization_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conna\Documents\GW_Modeling\GW_Homework\Working\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8F4924-E398-4DE4-AFA7-6B5AAF75FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401263E7-F778-4F1A-8CFC-F4D387CE8CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{E797DA87-9764-CF40-B10D-4CBD1F0C2290}"/>
   </bookViews>
@@ -19095,7 +19095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B842760C-4A3D-7C48-B8D8-B3990F9D725F}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="M4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -21766,7 +21766,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I32" sqref="I32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -24438,8 +24438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B7FEA8-679C-6245-B574-9BBD7BB6F993}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>